<commit_message>
Bulk excel template - Cypress(gangaraj testing)
Bulk excel template - Cypress(gangaraj testing)
</commit_message>
<xml_diff>
--- a/public/template/Cypress Ascendant Services LLC_sample_template.xlsx
+++ b/public/template/Cypress Ascendant Services LLC_sample_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(local)\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(dev)\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DD4E6C-6764-4A99-991A-7DE440A7BF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA63D4F-80A3-4A1D-90A3-E8A7CB7FCC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
     <t>Typing</t>
   </si>
   <si>
-    <t>Full Searchs</t>
+    <t>Full Search</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Sample template cypress process - search & typing added
Sample template cypress process - search & typing added
</commit_message>
<xml_diff>
--- a/public/template/Cypress Ascendant Services LLC_sample_template.xlsx
+++ b/public/template/Cypress Ascendant Services LLC_sample_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(dev)\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2469AC71-5C21-4C92-8500-D34ADFEE5720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8F3564-4A20-442E-8044-9C11BD17C09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -987,7 +987,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +1048,7 @@
         <v>45436</v>
       </c>
       <c r="B2" s="1">
-        <v>121356</v>
+        <v>1215356</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
role changes in vp and admin avp and ground abstractor and Partially Cancelled changes as done
role changes in vp and admin avp and ground abstractor and Partially Cancelled changes as done
</commit_message>
<xml_diff>
--- a/public/template/Cypress Ascendant Services LLC_sample_template.xlsx
+++ b/public/template/Cypress Ascendant Services LLC_sample_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tester\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35FE93F-E8A4-400A-8AF9-0BCE1E7AD483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29089575-BF41-46DA-9146-87DB93115C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="106">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -62,88 +62,298 @@
     <t>WIP</t>
   </si>
   <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Lob</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Commitment Typing</t>
+  </si>
+  <si>
+    <t>SIPL5316</t>
+  </si>
+  <si>
+    <t>SIPL5688</t>
+  </si>
+  <si>
+    <t>Current Owner Search</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Shelby</t>
+  </si>
+  <si>
+    <t>SIPL5317</t>
+  </si>
+  <si>
+    <t>SIPL6118</t>
+  </si>
+  <si>
+    <t>Full Search</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Legal and Vesting</t>
+  </si>
+  <si>
+    <t>Update Search</t>
+  </si>
+  <si>
+    <t>Two Owner Search</t>
+  </si>
+  <si>
     <t>Tier</t>
   </si>
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Lob</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>Search &amp; Typing</t>
-  </si>
-  <si>
-    <t>Typist</t>
-  </si>
-  <si>
-    <t>Typist QC</t>
-  </si>
-  <si>
-    <t>Acc10-001</t>
-  </si>
-  <si>
-    <t>SIPL5316</t>
-  </si>
-  <si>
-    <t>SIPL5688</t>
-  </si>
-  <si>
-    <t>SIPL0102</t>
-  </si>
-  <si>
-    <t>SIPL0103</t>
-  </si>
-  <si>
-    <t>Accurate</t>
-  </si>
-  <si>
-    <t>Current Owner Search</t>
-  </si>
-  <si>
-    <t>One Owner Equity</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>Adair</t>
-  </si>
-  <si>
-    <t>Acc10-002</t>
-  </si>
-  <si>
-    <t>Adams</t>
-  </si>
-  <si>
-    <t>Acc10-003</t>
-  </si>
-  <si>
-    <t>Equity</t>
-  </si>
-  <si>
     <t>Typing</t>
   </si>
   <si>
-    <t>EQ Prop 30yr</t>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Parcel Mapping</t>
+  </si>
+  <si>
+    <t>Autauga</t>
+  </si>
+  <si>
+    <t>Parcel Mapping Identification</t>
+  </si>
+  <si>
+    <t>Baldwin</t>
+  </si>
+  <si>
+    <t>I18-001</t>
+  </si>
+  <si>
+    <t>I18-002</t>
+  </si>
+  <si>
+    <t>Be18-001</t>
+  </si>
+  <si>
+    <t>Baseline Title</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>COS</t>
+  </si>
+  <si>
+    <t>Search(T1)</t>
+  </si>
+  <si>
+    <t>Be18-002</t>
+  </si>
+  <si>
+    <t>Be18-003</t>
+  </si>
+  <si>
+    <t>Bibb</t>
+  </si>
+  <si>
+    <t>Be18-004</t>
+  </si>
+  <si>
+    <t>Exam Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blount </t>
   </si>
   <si>
     <t>Typing(T1)</t>
   </si>
   <si>
-    <t>Typing(T2)</t>
-  </si>
-  <si>
-    <t>LnV</t>
-  </si>
-  <si>
-    <t>EQNow LNV with Tax</t>
+    <t>FM18-001</t>
+  </si>
+  <si>
+    <t>Ferr &amp; Mullin, P.C</t>
+  </si>
+  <si>
+    <t>FM18-002</t>
+  </si>
+  <si>
+    <t>FM18-003</t>
+  </si>
+  <si>
+    <t>FM18-004</t>
+  </si>
+  <si>
+    <t>Ferr &amp; Mullin, P.C - ABS</t>
+  </si>
+  <si>
+    <t>CBT18-001</t>
+  </si>
+  <si>
+    <t>Common Bond Title</t>
+  </si>
+  <si>
+    <t>CBTC18-001</t>
+  </si>
+  <si>
+    <t>California Best Title company</t>
+  </si>
+  <si>
+    <t>Farming</t>
+  </si>
+  <si>
+    <t>Re18-001</t>
+  </si>
+  <si>
+    <t>Reltco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search </t>
+  </si>
+  <si>
+    <t>Commercial Current Owner Search</t>
+  </si>
+  <si>
+    <t>ALShelby</t>
+  </si>
+  <si>
+    <t>Re18-002</t>
+  </si>
+  <si>
+    <t>Commercial Full Search</t>
+  </si>
+  <si>
+    <t>FLClay</t>
+  </si>
+  <si>
+    <t>Re18-003</t>
+  </si>
+  <si>
+    <t>SIPL4167</t>
+  </si>
+  <si>
+    <t>Commercial Update Search</t>
+  </si>
+  <si>
+    <t>Search(T2)</t>
+  </si>
+  <si>
+    <t>Re18-004</t>
+  </si>
+  <si>
+    <t>Residential Current Owner Search</t>
+  </si>
+  <si>
+    <t>Re18-005</t>
+  </si>
+  <si>
+    <t>Residential Full Search</t>
+  </si>
+  <si>
+    <t>Re18-006</t>
+  </si>
+  <si>
+    <t>Residential Update Search</t>
+  </si>
+  <si>
+    <t>WFG18-001</t>
+  </si>
+  <si>
+    <t>WFG Title</t>
+  </si>
+  <si>
+    <t>WFG18-002</t>
+  </si>
+  <si>
+    <t>WFG18-003</t>
+  </si>
+  <si>
+    <t>Beeline</t>
+  </si>
+  <si>
+    <t>ATA18-001</t>
+  </si>
+  <si>
+    <t>ATA National Title</t>
+  </si>
+  <si>
+    <t>ATA18-002</t>
+  </si>
+  <si>
+    <t>40 Years Search</t>
+  </si>
+  <si>
+    <t>ATA18-003</t>
+  </si>
+  <si>
+    <t>Current Owner Update</t>
+  </si>
+  <si>
+    <t>ATA18-004</t>
+  </si>
+  <si>
+    <t>40 Years Update</t>
+  </si>
+  <si>
+    <t>ATA18-005</t>
+  </si>
+  <si>
+    <t>30 Years Search</t>
+  </si>
+  <si>
+    <t>ATA18-006</t>
+  </si>
+  <si>
+    <t>60 Years Search</t>
+  </si>
+  <si>
+    <t>RPA18-001</t>
+  </si>
+  <si>
+    <t>Reliable Property Reports, Inc</t>
+  </si>
+  <si>
+    <t>RPA18-002</t>
+  </si>
+  <si>
+    <t>RPA18-003</t>
+  </si>
+  <si>
+    <t>Document Retrieval</t>
+  </si>
+  <si>
+    <t>RPA18-004</t>
+  </si>
+  <si>
+    <t>RPA18-005</t>
+  </si>
+  <si>
+    <t>RPA18-006</t>
+  </si>
+  <si>
+    <t>RPA18-007</t>
+  </si>
+  <si>
+    <t>Marketable Title</t>
+  </si>
+  <si>
+    <t>Municipality</t>
   </si>
 </sst>
 </file>
@@ -153,7 +363,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,19 +506,26 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,8 +711,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -625,8 +848,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -669,18 +905,28 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -718,14 +964,24 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Online Geo" xfId="42" xr:uid="{8C193209-4B5D-4D1F-AC45-410BCE3A9A4A}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1035,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,14 +1303,14 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="5" max="7" width="26.21875" customWidth="1"/>
     <col min="8" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1068,168 +1324,1556 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45635.0625</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>45550.0625</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45635.0625</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45634.770833333336</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45634.416666666664</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="I21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="K23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="D24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="I34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>45634.125</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>45635.0625</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>45557.0625</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="I36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>45635.0625</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>45635.0625</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>45561.0625</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>33</v>
+      <c r="I38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>45635.0625</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="E2:E3">
+    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>